<commit_message>
Character Dean function done
</commit_message>
<xml_diff>
--- a/public/templete/multiple_courses.xlsx
+++ b/public/templete/multiple_courses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Subject Code</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Credit</t>
-  </si>
-  <si>
-    <t>Reviewer (Staff ID)</t>
   </si>
 </sst>
 </file>
@@ -421,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,9 +464,7 @@
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
@@ -499,9 +494,7 @@
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>

</xml_diff>